<commit_message>
color with requested schedule
</commit_message>
<xml_diff>
--- a/solution_0.xlsx
+++ b/solution_0.xlsx
@@ -86,10 +86,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -136,12 +143,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -737,19 +750,19 @@
       <c r="W3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="X3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="Y3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="Z3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="AA3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="AB3" s="2" t="s">
+      <c r="X3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB3" s="4" t="s">
         <v>8</v>
       </c>
       <c r="AC3" s="1" t="s">
@@ -791,7 +804,7 @@
       <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -806,19 +819,19 @@
       <c r="F4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="I4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="J4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="K4" s="3" t="s">
         <v>12</v>
       </c>
       <c r="L4" s="2" t="s">
@@ -866,16 +879,16 @@
       <c r="Z4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="AA4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="AB4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="AC4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="AD4" s="1" t="s">
+      <c r="AA4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="AC4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="AD4" s="3" t="s">
         <v>8</v>
       </c>
       <c r="AE4" s="1" t="s">
@@ -944,7 +957,7 @@
       <c r="L5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M5" s="2" t="s">
+      <c r="M5" s="4" t="s">
         <v>8</v>
       </c>
       <c r="N5" s="1" t="s">
@@ -959,10 +972,10 @@
       <c r="Q5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="R5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="S5" s="2" t="s">
+      <c r="R5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="S5" s="4" t="s">
         <v>8</v>
       </c>
       <c r="T5" s="2" t="s">
@@ -980,16 +993,16 @@
       <c r="X5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="Y5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="Z5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="AA5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="AB5" s="2" t="s">
+      <c r="Y5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB5" s="4" t="s">
         <v>8</v>
       </c>
       <c r="AC5" s="1" t="s">
@@ -1031,7 +1044,7 @@
       <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -1070,7 +1083,7 @@
       <c r="N6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="O6" s="1" t="s">
+      <c r="O6" s="3" t="s">
         <v>8</v>
       </c>
       <c r="P6" s="1" t="s">
@@ -1091,7 +1104,7 @@
       <c r="U6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="V6" s="1" t="s">
+      <c r="V6" s="3" t="s">
         <v>13</v>
       </c>
       <c r="W6" s="1" t="s">
@@ -1106,10 +1119,10 @@
       <c r="Z6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="AA6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="AB6" s="2" t="s">
+      <c r="AA6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="AB6" s="4" t="s">
         <v>10</v>
       </c>
       <c r="AC6" s="1" t="s">
@@ -1181,25 +1194,25 @@
       <c r="K7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L7" s="2" t="s">
+      <c r="L7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="M7" s="2" t="s">
+      <c r="M7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="N7" s="1" t="s">
+      <c r="N7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="P7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="R7" s="1" t="s">
+      <c r="O7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="P7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="R7" s="3" t="s">
         <v>8</v>
       </c>
       <c r="S7" s="2" t="s">
@@ -1298,13 +1311,13 @@
       <c r="J8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K8" s="1" t="s">
+      <c r="K8" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="L8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="M8" s="2" t="s">
+      <c r="L8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="M8" s="4" t="s">
         <v>8</v>
       </c>
       <c r="N8" s="1" t="s">
@@ -1322,7 +1335,7 @@
       <c r="R8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="S8" s="2" t="s">
+      <c r="S8" s="4" t="s">
         <v>8</v>
       </c>
       <c r="T8" s="2" t="s">
@@ -1352,10 +1365,10 @@
       <c r="AB8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="AC8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="AD8" s="1" t="s">
+      <c r="AC8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="AD8" s="3" t="s">
         <v>8</v>
       </c>
       <c r="AE8" s="1" t="s">
@@ -1391,13 +1404,13 @@
       <c r="A9" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E9" s="2" t="s">
@@ -1424,19 +1437,19 @@
       <c r="L9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="M9" s="2" t="s">
+      <c r="M9" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="N9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="O9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="P9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q9" s="1" t="s">
+      <c r="N9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="O9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="P9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q9" s="3" t="s">
         <v>8</v>
       </c>
       <c r="R9" s="1" t="s">

</xml_diff>